<commit_message>
correction typos suite review 97cb5962765b8e83db398b152ed3b4614f0dc8c3
</commit_message>
<xml_diff>
--- a/ig/profiling_researchstudy/StructureDefinition-eclaire-contact-type.xlsx
+++ b/ig/profiling_researchstudy/StructureDefinition-eclaire-contact-type.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-07-04T19:15:23+00:00</t>
+    <t>2023-07-05T07:22:55+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -72,7 +72,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Extension créée dans le cadre du projet ECLAIRE qui indique le type de Contact! : Public ou Scientific</t>
+    <t>Extension créée dans le cadre du projet ECLAIRE qui indique le type de Contact : Public ou Scientific</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>